<commit_message>
added test_case data and testing script
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ts-jawad.arman\Desktop\my_commit\home_task\Change-Password\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0018F0AC-E73D-4A22-A855-F7413FBEE987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86244A64-AA9E-4F33-9B81-5CFECF4F25E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2033,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="3" t="s">
         <v>165</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="3" t="s">
         <v>167</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="3" t="s">
         <v>169</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="3" t="s">
         <v>172</v>
       </c>
@@ -2324,18 +2324,25 @@
       <c r="F21" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22" s="3" t="s">
+      <c r="G21" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B22" s="20"/>
+      <c r="C22" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F22" s="4" t="b">
+      <c r="F22" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2358,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1DE413-6706-4A1D-9967-0D46A29EE5BA}">
   <dimension ref="B1:G119"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>